<commit_message>
Updated Excel sheet with new data row
</commit_message>
<xml_diff>
--- a/python/Wave1.xlsx
+++ b/python/Wave1.xlsx
@@ -718,7 +718,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AB279"/>
+  <dimension ref="A1:AB280"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
@@ -2665,6 +2665,148 @@
         </is>
       </c>
     </row>
+    <row r="280">
+      <c r="A280" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="B280" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="C280" t="inlineStr">
+        <is>
+          <t>Chennai</t>
+        </is>
+      </c>
+      <c r="D280" t="inlineStr">
+        <is>
+          <t>Tamil Nadu</t>
+        </is>
+      </c>
+      <c r="E280" t="inlineStr">
+        <is>
+          <t>600117</t>
+        </is>
+      </c>
+      <c r="F280" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="G280" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="H280" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="I280" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="J280" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="K280" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="L280" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="M280" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="N280" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="O280" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="P280" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="Q280" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="R280" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="S280" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="T280" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="U280" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="V280" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="W280" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="X280" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="Y280" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="Z280" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AA280" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AB280" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:AB17"/>
   <conditionalFormatting sqref="P17">

</xml_diff>